<commit_message>
regen sval data to filter save games
</commit_message>
<xml_diff>
--- a/data/calcs/save_calcs/global_conglomerate_mu_std.xlsx
+++ b/data/calcs/save_calcs/global_conglomerate_mu_std.xlsx
@@ -482,28 +482,28 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2.979492567514982</v>
+        <v>1.465341735336888</v>
       </c>
       <c r="C2" t="n">
-        <v>30.80430383687446</v>
+        <v>17.30416868637906</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1837886216826212</v>
+        <v>1.019631604459525</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.3336446416063507</v>
+        <v>-0.2947164323800291</v>
       </c>
       <c r="F2" t="n">
-        <v>1.98171063896023</v>
+        <v>1.22200678623364</v>
       </c>
       <c r="G2" t="n">
-        <v>2.120126079850572</v>
+        <v>1.207222491517208</v>
       </c>
       <c r="H2" t="n">
-        <v>5.651568215425325</v>
+        <v>8.792777508482793</v>
       </c>
       <c r="I2" t="n">
-        <v>6.771694295275897</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3">
@@ -513,28 +513,28 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>3.800079429817507</v>
+        <v>2.019693578208169</v>
       </c>
       <c r="C3" t="n">
-        <v>28.77523990190277</v>
+        <v>9.195957851124549</v>
       </c>
       <c r="D3" t="n">
-        <v>3.764980410717235</v>
+        <v>4.270133340904041</v>
       </c>
       <c r="E3" t="n">
-        <v>1.750447669744413</v>
+        <v>0.9703013987511284</v>
       </c>
       <c r="F3" t="n">
-        <v>2.204417058247611</v>
+        <v>1.085512506669432</v>
       </c>
       <c r="G3" t="n">
-        <v>1.796124762593388</v>
+        <v>0.5297969353132786</v>
       </c>
       <c r="H3" t="n">
-        <v>2.937865201782139</v>
+        <v>0.5297969353132786</v>
       </c>
       <c r="I3" t="n">
-        <v>1.873261141842476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -544,28 +544,28 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>3.04029272858784</v>
+        <v>1.475273418925345</v>
       </c>
       <c r="C4" t="n">
-        <v>32.38973748032166</v>
+        <v>17.7246790299572</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.1246223886312386</v>
+        <v>0.9864479315263909</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.294813428073012</v>
+        <v>-0.3031383737517832</v>
       </c>
       <c r="F4" t="n">
-        <v>1.934518997574778</v>
+        <v>1.187351402757965</v>
       </c>
       <c r="G4" t="n">
-        <v>2.237373952261414</v>
+        <v>1.245601521635759</v>
       </c>
       <c r="H4" t="n">
-        <v>5.73896949325618</v>
+        <v>8.754398478364241</v>
       </c>
       <c r="I4" t="n">
-        <v>6.976343445517593</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
@@ -575,28 +575,28 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>3.859418171168862</v>
+        <v>2.026162321730315</v>
       </c>
       <c r="C5" t="n">
-        <v>29.91140010449857</v>
+        <v>9.413694306879455</v>
       </c>
       <c r="D5" t="n">
-        <v>3.743783211116772</v>
+        <v>4.273531832562288</v>
       </c>
       <c r="E5" t="n">
-        <v>1.757610313947826</v>
+        <v>0.9636063076605779</v>
       </c>
       <c r="F5" t="n">
-        <v>2.105083633887729</v>
+        <v>1.05410889547806</v>
       </c>
       <c r="G5" t="n">
-        <v>1.89302778538848</v>
+        <v>0.5609770710404465</v>
       </c>
       <c r="H5" t="n">
-        <v>2.983413554889751</v>
+        <v>0.5609770710404464</v>
       </c>
       <c r="I5" t="n">
-        <v>1.77371535560166</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -606,28 +606,28 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.167209816938242</v>
+        <v>1.563603440470801</v>
       </c>
       <c r="C6" t="n">
-        <v>32.32339569503118</v>
+        <v>18.29923042100498</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.07427077046871856</v>
+        <v>0.9637845178813943</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.3233956950311809</v>
+        <v>-0.3198279764599366</v>
       </c>
       <c r="F6" t="n">
-        <v>2.007523637095152</v>
+        <v>1.234721593481213</v>
       </c>
       <c r="G6" t="n">
-        <v>2.232347616173808</v>
+        <v>1.279764599366229</v>
       </c>
       <c r="H6" t="n">
-        <v>5.663327298330316</v>
+        <v>8.72023540063377</v>
       </c>
       <c r="I6" t="n">
-        <v>6.895674914504124</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
@@ -637,28 +637,28 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4.020823103252575</v>
+        <v>2.204438451590914</v>
       </c>
       <c r="C7" t="n">
-        <v>29.93746099773191</v>
+        <v>10.67865166581983</v>
       </c>
       <c r="D7" t="n">
-        <v>3.805370412341394</v>
+        <v>4.385752075066329</v>
       </c>
       <c r="E7" t="n">
-        <v>1.815286801188645</v>
+        <v>1.019737640802872</v>
       </c>
       <c r="F7" t="n">
-        <v>2.177002865735982</v>
+        <v>1.108306638962272</v>
       </c>
       <c r="G7" t="n">
-        <v>1.859873386579374</v>
+        <v>0.6493079779011089</v>
       </c>
       <c r="H7" t="n">
-        <v>2.974183619009204</v>
+        <v>0.6493079779011089</v>
       </c>
       <c r="I7" t="n">
-        <v>1.828074353039111</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -668,28 +668,28 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3.010917598128412</v>
+        <v>1.490718124084025</v>
       </c>
       <c r="C8" t="n">
-        <v>31.6454380036392</v>
+        <v>17.66927210552027</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.04232735464864396</v>
+        <v>0.9201270151441133</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.2955549779048609</v>
+        <v>-0.3094772838299951</v>
       </c>
       <c r="F8" t="n">
-        <v>1.922623689454987</v>
+        <v>1.140693698094773</v>
       </c>
       <c r="G8" t="n">
-        <v>2.213326401524998</v>
+        <v>1.256228627259404</v>
       </c>
       <c r="H8" t="n">
-        <v>5.725587037518412</v>
+        <v>8.743771372740596</v>
       </c>
       <c r="I8" t="n">
-        <v>6.938913439043411</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -699,28 +699,28 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3.851637735192067</v>
+        <v>2.075954932242621</v>
       </c>
       <c r="C9" t="n">
-        <v>29.59691237540997</v>
+        <v>9.857303339678452</v>
       </c>
       <c r="D9" t="n">
-        <v>3.668700975288921</v>
+        <v>4.172053473022855</v>
       </c>
       <c r="E9" t="n">
-        <v>1.762288106679183</v>
+        <v>0.9699733740136783</v>
       </c>
       <c r="F9" t="n">
-        <v>2.094283503239229</v>
+        <v>1.03882138644175</v>
       </c>
       <c r="G9" t="n">
-        <v>1.858748179386223</v>
+        <v>0.5894703072243467</v>
       </c>
       <c r="H9" t="n">
-        <v>2.961795266157456</v>
+        <v>0.5894703072243467</v>
       </c>
       <c r="I9" t="n">
-        <v>1.791065105725621</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>